<commit_message>
added results from NL to test case generation through LLM
</commit_message>
<xml_diff>
--- a/Results/Results_EGAS.xlsx
+++ b/Results/Results_EGAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FOKUS\LESS_2\SE_26\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5DE8AC1-5EFD-4B96-AA7A-BF90FA708AC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5527409-458F-44F7-B126-2ABBEE8FDF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="3" xr2:uid="{34E2BE8E-85C9-4BDF-A9B0-7DEAF13743E9}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" firstSheet="3" activeTab="3" xr2:uid="{34E2BE8E-85C9-4BDF-A9B0-7DEAF13743E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Exp_NL_TO_LESS" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="102">
   <si>
     <t>LESS Requirement Generation</t>
   </si>
@@ -1146,6 +1146,387 @@
   </si>
   <si>
     <t>Others (incorrect expressions added)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Grammar in NLP
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Results/test_generation/nlp_test_generation/1_GPT-5/prompt_4_nlp_test_gen_gpt5.txt)</t>
+    </r>
+  </si>
+  <si>
+    <t>9 (50%)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">6
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>line 10: "high", "confirm" obj attr. and verb misclassified
+line 13: "malicious" and "detect" used as states 
+line 14: "malicious" and "transmit" used as states
+line15:"malicious" and ""transmit" used as states
+line 16: "drop" verb used as state
+line 18: "transfer" used as a state</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">4
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>line 9: missing "signals", "actuator" test objects
+line 10: missed "state" test obj
+line 14: missing "being_transmitted" test obj
+line 18: "signals" missing as test obj</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">3
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>line 9: hallucinnated "actuator_signals"
+line 16: no such states as "malicious_detected"
+line 18: "from_navigation”, “transfer”, "Whitelist" do not exist</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">8
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>line 10: model added PRE and POST state
+line 11: model added PRE and POST state
+line 13: model added PRE and POST state
+line 14: model added PRE and POST state
+line 15: model added PRE and POST state
+line 16: model added PRE and POST state
+line 17: model added PRE and POST state
+line 18: model added PRE and POST state</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Grammar in NLP
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Results/test_generation/nlp_test_generation/2_Llama4/prompt_5_nlp_test_gen_llama4.txt)</t>
+    </r>
+  </si>
+  <si>
+    <t>9 (60%)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">5
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Line 4: "plausability" used as a state
+Line 5: "plausability" used as a state
+Line 6: "plausability" used as a state
+Line 8: "plausability" used as a state
+Line 11:"protect" "integrity" used as state</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">6
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Line 4: "plausability" not included as test object
+line 5: "plausability" not included as test object
+line 6: "plausability" not included as test object
+line 8: "actuator" and "signals" not included in test obj
+line 11: "integrity" "lamp_switch_on_request" missing 
+line 13: test object does not have "being_transmitted"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">5
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Line 4: "check" does not exist in vocab
+Line 5: "check" does not exist in vocab
+line 6:  "check" does not exist in vocab
+line 8: "check" and "actuator_signals" do not exist in vocab
+line 11: no such object as "lamp_switch"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">6
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>line 4: model added  POST state
+line 5: model added  POST state
+line 6: model added  POST state
+line 8: model added  POST state
+line 11: model added POST state
+line 13: model added POST state</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Grammar in NLP
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Results/test_generation/nlp_test_generation/3_DeepSeek/prompt_4_nlp_test_gen_deepseek.txt)</t>
+    </r>
+  </si>
+  <si>
+    <t>11 (50%)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">4
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Line 12: "Detected" is not a state
+Line 14: "spoofing” is a object attribute but used as object
+Line 18: “malicious”, "detected" are object attributes and not a state
+Line 19: "gernerated" is verb but used as state</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">9
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Line 7: “torque_signals_affecting_requirements_of_other_ECUs”  missing as test object
+Line 9: Test object missing "actuator"
+Line 10: test object does not have “driving_torque” and “state”
+Line 12: "driving_torque" missing as test object
+LIne 14: "lamp_switch_on_Request" missing in test object
+Line 16: missing "being_transmitted"
+Line 19: missing "reqest" as test object
+Line 20: “lamp_switch_on_request” in test object is missing
+line 21: missing "signals" in the test object list</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">9
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Line 7: no such term as "torque_related_signals"
+Line 9: no such term as "actuator_signals"
+Line 10: “high_driving_torque_state” no such term
+Line 12: no such term as "high_driving_torque"
+Line 14: “lamp_switch” object does not exist
+Line 18: no such term as "dropped" in vocab 
+Line 19: no such term as "requested"
+Line 20: no such term as "transmitted"
+line 21: no such term as "whitelist" in vocab</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">4
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Line 18: PRE and POST state not explicit from req. but model added them anyway
+line 19: model added PRE and POST state
+line 20: model added PRE and POST state
+line 21: model added PRE and POST state</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1652,7 +2033,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1736,138 +2117,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1876,9 +2140,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1887,8 +2148,131 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2232,73 +2616,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12">
-      <c r="B1" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="53"/>
+      <c r="B1" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="66"/>
     </row>
     <row r="2" spans="2:12" ht="70.5" customHeight="1">
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
     </row>
     <row r="3" spans="2:12" ht="80.25" customHeight="1">
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
     </row>
     <row r="4" spans="2:12" ht="14.65" customHeight="1">
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58" t="s">
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
     </row>
     <row r="5" spans="2:12" ht="30.75">
-      <c r="B5" s="57"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="42"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="55"/>
       <c r="E5" s="32" t="s">
         <v>8</v>
       </c>
@@ -2322,13 +2706,13 @@
       </c>
     </row>
     <row r="6" spans="2:12" ht="60.75">
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="59" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="89" t="s">
+      <c r="D6" s="90" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="26">
@@ -2354,23 +2738,23 @@
       </c>
     </row>
     <row r="7" spans="2:12">
-      <c r="B7" s="46"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="45"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="58"/>
     </row>
     <row r="8" spans="2:12" ht="165" customHeight="1">
-      <c r="B8" s="47"/>
+      <c r="B8" s="60"/>
       <c r="C8" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="89" t="s">
+      <c r="D8" s="90" t="s">
         <v>25</v>
       </c>
       <c r="E8" s="21">
@@ -2396,23 +2780,23 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B9" s="47"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="45"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="58"/>
     </row>
     <row r="10" spans="2:12" ht="91.5">
-      <c r="B10" s="47"/>
+      <c r="B10" s="60"/>
       <c r="C10" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="89" t="s">
+      <c r="D10" s="90" t="s">
         <v>31</v>
       </c>
       <c r="E10" s="21">
@@ -2452,41 +2836,41 @@
     <row r="12" spans="2:12"/>
     <row r="13" spans="2:12"/>
     <row r="14" spans="2:12" ht="14.65" customHeight="1">
-      <c r="B14" s="60" t="s">
+      <c r="B14" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="61"/>
-      <c r="L14" s="62"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="74"/>
+      <c r="I14" s="74"/>
+      <c r="J14" s="74"/>
+      <c r="K14" s="74"/>
+      <c r="L14" s="75"/>
     </row>
     <row r="15" spans="2:12">
-      <c r="B15" s="63" t="s">
+      <c r="B15" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="64"/>
-      <c r="J15" s="64"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="65"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="77"/>
+      <c r="H15" s="77"/>
+      <c r="I15" s="77"/>
+      <c r="J15" s="77"/>
+      <c r="K15" s="77"/>
+      <c r="L15" s="78"/>
     </row>
     <row r="16" spans="2:12">
       <c r="B16" s="13"/>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="36"/>
+      <c r="D16" s="49"/>
       <c r="E16" s="15" t="s">
         <v>37</v>
       </c>
@@ -2513,13 +2897,13 @@
       </c>
     </row>
     <row r="17" spans="2:12" ht="30.75">
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="38"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="24" t="s">
         <v>45</v>
       </c>
@@ -2546,11 +2930,11 @@
       </c>
     </row>
     <row r="18" spans="2:12" ht="30.75">
-      <c r="B18" s="47"/>
-      <c r="C18" s="39" t="s">
+      <c r="B18" s="60"/>
+      <c r="C18" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="40"/>
+      <c r="D18" s="53"/>
       <c r="E18" s="24" t="s">
         <v>48</v>
       </c>
@@ -2577,11 +2961,11 @@
       </c>
     </row>
     <row r="19" spans="2:12" ht="30.75">
-      <c r="B19" s="47"/>
-      <c r="C19" s="39" t="s">
+      <c r="B19" s="60"/>
+      <c r="C19" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="40"/>
+      <c r="D19" s="53"/>
       <c r="E19" s="24" t="s">
         <v>51</v>
       </c>
@@ -2634,41 +3018,41 @@
       <c r="L21" s="17"/>
     </row>
     <row r="22" spans="2:12">
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="61"/>
-      <c r="G22" s="61"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="61"/>
-      <c r="K22" s="61"/>
-      <c r="L22" s="62"/>
+      <c r="C22" s="74"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="74"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="74"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="74"/>
+      <c r="K22" s="74"/>
+      <c r="L22" s="75"/>
     </row>
     <row r="23" spans="2:12" ht="14.65" customHeight="1">
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="50"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="62"/>
+      <c r="L23" s="63"/>
     </row>
     <row r="24" spans="2:12">
       <c r="B24" s="13"/>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="36"/>
+      <c r="D24" s="49"/>
       <c r="E24" s="15" t="s">
         <v>37</v>
       </c>
@@ -2695,13 +3079,13 @@
       </c>
     </row>
     <row r="25" spans="2:12" ht="30.75">
-      <c r="B25" s="46" t="s">
+      <c r="B25" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="38"/>
+      <c r="D25" s="51"/>
       <c r="E25" s="24" t="s">
         <v>54</v>
       </c>
@@ -2728,11 +3112,11 @@
       </c>
     </row>
     <row r="26" spans="2:12">
-      <c r="B26" s="47"/>
-      <c r="C26" s="39" t="s">
+      <c r="B26" s="60"/>
+      <c r="C26" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="40"/>
+      <c r="D26" s="53"/>
       <c r="E26" s="23">
         <v>0</v>
       </c>
@@ -2759,11 +3143,11 @@
       </c>
     </row>
     <row r="27" spans="2:12">
-      <c r="B27" s="47"/>
-      <c r="C27" s="39" t="s">
+      <c r="B27" s="60"/>
+      <c r="C27" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="40"/>
+      <c r="D27" s="53"/>
       <c r="E27" s="23">
         <v>0</v>
       </c>
@@ -2830,7 +3214,7 @@
   <dimension ref="C1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:J3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
@@ -2848,121 +3232,121 @@
     <row r="1" spans="3:10" ht="15"/>
     <row r="2" spans="3:10" ht="15"/>
     <row r="3" spans="3:10" ht="15">
-      <c r="C3" s="80" t="s">
+      <c r="C3" s="79" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="80"/>
-      <c r="E3" s="80"/>
-      <c r="F3" s="80"/>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
     </row>
     <row r="4" spans="3:10" ht="14.65" customHeight="1">
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="74" t="s">
+      <c r="E4" s="81" t="s">
         <v>56</v>
       </c>
-      <c r="F4" s="75" t="s">
+      <c r="F4" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="G4" s="77" t="s">
+      <c r="G4" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-      <c r="J4" s="77"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
     </row>
     <row r="5" spans="3:10" ht="14.65" customHeight="1">
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="78" t="s">
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="78" t="s">
+      <c r="H5" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="79" t="s">
+      <c r="I5" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="J5" s="79" t="s">
+      <c r="J5" s="41" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="6" spans="3:10" ht="96" customHeight="1">
-      <c r="C6" s="72" t="s">
+      <c r="C6" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="73" t="s">
+      <c r="D6" s="39" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="27">
         <v>18</v>
       </c>
-      <c r="F6" s="69" t="s">
+      <c r="F6" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="82">
-        <v>0</v>
-      </c>
-      <c r="H6" s="81" t="s">
+      <c r="G6" s="43">
+        <v>0</v>
+      </c>
+      <c r="H6" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="I6" s="82">
-        <v>0</v>
-      </c>
-      <c r="J6" s="81" t="s">
+      <c r="I6" s="43">
+        <v>0</v>
+      </c>
+      <c r="J6" s="42" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="7" spans="3:10" ht="60.75">
-      <c r="C7" s="68" t="s">
+      <c r="C7" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="69" t="s">
+      <c r="D7" s="37" t="s">
         <v>67</v>
       </c>
       <c r="E7" s="23">
         <v>15</v>
       </c>
-      <c r="F7" s="69" t="s">
+      <c r="F7" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="82">
-        <v>0</v>
-      </c>
-      <c r="H7" s="81" t="s">
+      <c r="G7" s="43">
+        <v>0</v>
+      </c>
+      <c r="H7" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="I7" s="82">
-        <v>0</v>
-      </c>
-      <c r="J7" s="82">
+      <c r="I7" s="43">
+        <v>0</v>
+      </c>
+      <c r="J7" s="43">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="3:10" ht="106.5">
-      <c r="C8" s="83" t="s">
+      <c r="C8" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="69" t="s">
+      <c r="D8" s="37" t="s">
         <v>71</v>
       </c>
       <c r="E8" s="23">
         <v>21</v>
       </c>
-      <c r="F8" s="69" t="s">
+      <c r="F8" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="G8" s="81" t="s">
+      <c r="G8" s="42" t="s">
         <v>73</v>
       </c>
       <c r="H8" s="22" t="s">
@@ -2989,12 +3373,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="C3:J3"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:J4"/>
-    <mergeCell ref="C3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3020,24 +3404,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:10">
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
     <row r="2" spans="3:10">
-      <c r="C2" s="67" t="s">
+      <c r="C2" s="87" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -3093,126 +3477,167 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC2638F1-068A-4418-89AB-4E730123006C}">
-  <dimension ref="B1:I18"/>
+  <dimension ref="B1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
     <col min="2" max="2" width="38.140625" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" customWidth="1"/>
-    <col min="9" max="9" width="25" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="6" max="6" width="47.28515625" customWidth="1"/>
+    <col min="7" max="7" width="63.140625" customWidth="1"/>
+    <col min="8" max="8" width="36.5703125" customWidth="1"/>
+    <col min="9" max="9" width="53" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15"/>
     <row r="2" spans="2:9" ht="15"/>
-    <row r="3" spans="2:9" ht="15">
-      <c r="B3" s="88" t="s">
+    <row r="3" spans="2:9" ht="15"/>
+    <row r="4" spans="2:9" ht="15">
+      <c r="B4" s="88" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-    </row>
-    <row r="4" spans="2:9" ht="15">
-      <c r="B4" s="70" t="s">
+      <c r="C4" s="88"/>
+      <c r="D4" s="88"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
+    </row>
+    <row r="5" spans="2:9" ht="15">
+      <c r="B5" s="80" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C5" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="84" t="s">
+      <c r="D5" s="89" t="s">
         <v>82</v>
       </c>
-      <c r="E4" s="70" t="s">
+      <c r="E5" s="80" t="s">
         <v>57</v>
       </c>
-      <c r="F4" s="77" t="s">
+      <c r="F5" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="77"/>
-      <c r="H4" s="77"/>
-      <c r="I4" s="77"/>
-    </row>
-    <row r="5" spans="2:9" ht="30.95" customHeight="1">
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="85" t="s">
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+    </row>
+    <row r="6" spans="2:9" ht="30.95" customHeight="1">
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="85" t="s">
+      <c r="G6" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="86" t="s">
+      <c r="H6" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="87" t="s">
+      <c r="I6" s="47" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="15">
-      <c r="B6" s="69" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="69" t="s">
+    <row r="7" spans="2:9" ht="145.5" customHeight="1">
+      <c r="B7" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="69"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
-    </row>
-    <row r="7" spans="2:9">
-      <c r="B7" s="69"/>
-      <c r="C7" s="69" t="s">
+      <c r="D7" s="43">
+        <v>18</v>
+      </c>
+      <c r="E7" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="I7" s="42" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="153.75" customHeight="1">
+      <c r="B8" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-    </row>
-    <row r="8" spans="2:9">
-      <c r="B8" s="69"/>
-      <c r="C8" s="69" t="s">
+      <c r="D8" s="43">
+        <v>15</v>
+      </c>
+      <c r="E8" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="I8" s="42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="192.75" customHeight="1">
+      <c r="B9" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-    </row>
-    <row r="9" spans="2:9" ht="15"/>
-    <row r="15" spans="2:9" ht="15"/>
+      <c r="D9" s="43">
+        <v>21</v>
+      </c>
+      <c r="E9" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="15"/>
     <row r="16" spans="2:9" ht="15"/>
-    <row r="18" ht="15"/>
+    <row r="17" ht="15"/>
+    <row r="19" ht="15"/>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3236,20 +3661,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5">
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
     </row>
     <row r="2" spans="2:5">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="87" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="10" t="s">

</xml_diff>

<commit_message>
added detailed logs for EGAS
</commit_message>
<xml_diff>
--- a/Results/Results_EGAS.xlsx
+++ b/Results/Results_EGAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FOKUS\LESS_2\SE_26\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5527409-458F-44F7-B126-2ABBEE8FDF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{68C81AD9-4935-41ED-977F-1A590C39E29D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" firstSheet="3" activeTab="3" xr2:uid="{34E2BE8E-85C9-4BDF-A9B0-7DEAF13743E9}"/>
   </bookViews>
@@ -40,9 +40,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="102">
-  <si>
-    <t>LESS Requirement Generation</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="125">
+  <si>
+    <t>NL TO LESS Requirement Generation</t>
   </si>
   <si>
     <r>
@@ -71,7 +71,8 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">. All RUN details and results are in </t>
+      <t xml:space="preserve">. 
+All RUN details and results are in </t>
     </r>
     <r>
       <rPr>
@@ -81,9 +82,10 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">/Results/req_generation/&lt;model_name&gt;
-</t>
-    </r>
+      <t>/Results/logs/req_generation/&lt;model_name&gt;</t>
+    </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -92,39 +94,39 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Prompt </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>used</t>
+      <t xml:space="preserve">Evaluation dataset (ground truth): </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Results/logs/0_Ground_Truth/Requirement_generation
+</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/Prompts/EGAS/prompt_14.txt</t>
-    </r>
-  </si>
-  <si>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Total NL-LESS pair in Eval. set: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">30
+</t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -133,63 +135,22 @@
         <rFont val="Calibri"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Evaluation dataset: </t>
+      <t>Total NL requirements</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> given to model for generation: 25
+</t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FF4472C4"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Results/logs/0_Ground_Truth/Requirement_generation
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Total NL-LESS pair in Eval. set: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">30
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Total NL requirements</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> given to model for generation: 25
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <scheme val="minor"/>
@@ -220,6 +181,12 @@
   </si>
   <si>
     <t>Syntactically Incorrect Generations</t>
+  </si>
+  <si>
+    <t>RUN</t>
+  </si>
+  <si>
+    <t>Results location</t>
   </si>
   <si>
     <t>Exact Matches</t>
@@ -447,6 +414,12 @@
       </rPr>
       <t>(Line 13: malformed conditional)</t>
     </r>
+  </si>
+  <si>
+    <t>Run 1</t>
+  </si>
+  <si>
+    <t>Results/logs/requirement_generation/indirect_prompts/4_gpt5/prompt14/run1__TAKEN/prompt_14_indirect_gpt.docx</t>
   </si>
   <si>
     <t>LLAMA4</t>
@@ -603,6 +576,12 @@
     </r>
   </si>
   <si>
+    <t>Run 2</t>
+  </si>
+  <si>
+    <t>Results/logs/requirement_generation/indirect_prompts/5_llama4/Prompt15_TAKEN/RUN2_TAKEN/prompt_14_indirect_llama4.docx</t>
+  </si>
+  <si>
     <t>DeepSeekV3.2</t>
   </si>
   <si>
@@ -711,6 +690,9 @@
     </r>
   </si>
   <si>
+    <t>/Results/logs/requirement_generation/indirect_prompts/3_deepseekV3/prompt14/run2__TAKEN/prompt_14_indirect_deepseek.docx</t>
+  </si>
+  <si>
     <t>Error Breakdown</t>
   </si>
   <si>
@@ -915,7 +897,87 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Runs: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The entries here are </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>best results from 3 runs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for all models
+Detailed results from all runs are organised per model in location: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Results/logs/test_generation/less_test_generation/EGAS/&lt;model_name&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ground Truth:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> For corresponding models, LESS requirements generated correctly by that model was provided as LESS input to generate test cases
+Ground truth is organised in each model folder as "Deterministic". The same LESS requirement given to individual models to generate test cases were given to a python script to generate test cases, this is then considerd as base line. 
+All locations in table below</t>
+    </r>
+  </si>
+  <si>
     <t>LESS to Test Case Generation</t>
+  </si>
+  <si>
+    <t>Ground Truth location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUN </t>
   </si>
   <si>
     <t>Total LESS Specifications</t>
@@ -1016,6 +1078,15 @@
     </r>
   </si>
   <si>
+    <t>Results/logs/test_generation/less_test_generation/EGAS/1_GPT5/Deterministic/generated_testcases_deterministic_ZSS01_GPT5_GT.docx</t>
+  </si>
+  <si>
+    <t>RUN 1</t>
+  </si>
+  <si>
+    <t>Results/logs/test_generation/less_test_generation/EGAS/1_GPT5/Non_deterministic/RUN1_TAKEN/AUTO_generated_gpt5.docx</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1045,6 +1116,12 @@
   <si>
     <t>1
 Line 14</t>
+  </si>
+  <si>
+    <t>Results/logs/test_generation/less_test_generation/EGAS/3_llama4/Deterministic/generated_testcases_deterministic_ZSS01__llama4_GT.docx</t>
+  </si>
+  <si>
+    <t>Results/logs/test_generation/less_test_generation/EGAS/3_llama4/NonDeterministic/RUN1_TAKEN/AUTO_generated_llama4.docx</t>
   </si>
   <si>
     <r>
@@ -1124,6 +1201,12 @@
 </t>
   </si>
   <si>
+    <t>Results/logs/test_generation/less_test_generation/EGAS/2_DeepSeek/Deterministic/generated_testcases_deterministic_ZSS01_DeepSeek_GT.docx</t>
+  </si>
+  <si>
+    <t>Results/logs/test_generation/less_test_generation/EGAS/2_DeepSeek/NonDeterministic/RUN1_TAKEN/AUTO_generated_deepseek.docx</t>
+  </si>
+  <si>
     <t>Model Hallucinations</t>
   </si>
   <si>
@@ -1137,6 +1220,79 @@
   </si>
   <si>
     <t>LLAMA-7B</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Runs: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The entries here are </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>best results from 3 runs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for all models
+Detailed results from all runs are organised per model in location: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Results/logs/test_generation/nlp_test_generation/&lt;model_name&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ground Truth:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> For corresponding models, NL equivalent of the LESS requirements generated correctly by that model was provided as NL input to generate test cases
+Ground truth is organised in each model folder as "Deterministic". </t>
+    </r>
   </si>
   <si>
     <t>NLP to Test Case Generation</t>
@@ -1273,6 +1429,9 @@
     </r>
   </si>
   <si>
+    <t>Results/logs/test_generation/nlp_test_generation/1_GPT-5/RUN1_TAKEN/AUTO_generated_gpt5.docx</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1397,6 +1556,9 @@
 line 11: model added POST state
 line 13: model added POST state</t>
     </r>
+  </si>
+  <si>
+    <t>Results/logs/test_generation/nlp_test_generation/2_Llama4/RUN1/AUTO_generated_llama4.docx</t>
   </si>
   <si>
     <r>
@@ -1528,12 +1690,15 @@
 line 21: model added PRE and POST state</t>
     </r>
   </si>
+  <si>
+    <t>Results/logs/test_generation/nlp_test_generation/3_DeepSeek/RUN1_TAKEN/AUTO_generated_deepseek.docx</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1607,8 +1772,15 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1679,8 +1851,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1997,15 +2181,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -2018,12 +2193,50 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -2033,7 +2246,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -2066,12 +2279,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2096,17 +2303,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2128,10 +2326,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2148,6 +2342,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2166,21 +2366,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2199,30 +2387,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2241,24 +2408,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2268,13 +2423,129 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="16" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="17" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2593,10 +2864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79AAD88-F198-489C-B36B-918A39BD4411}">
-  <dimension ref="B1:L28"/>
+  <dimension ref="B1:M28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -2611,218 +2882,253 @@
     <col min="9" max="9" width="32" customWidth="1"/>
     <col min="10" max="10" width="25.7109375" customWidth="1"/>
     <col min="11" max="11" width="39.42578125" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
-    <col min="13" max="13" width="113.28515625" customWidth="1"/>
+    <col min="12" max="12" width="45.5703125" customWidth="1"/>
+    <col min="13" max="13" width="127.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12">
-      <c r="B1" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="66"/>
-    </row>
-    <row r="2" spans="2:12" ht="70.5" customHeight="1">
-      <c r="B2" s="67" t="s">
+    <row r="1" spans="2:13">
+      <c r="B1" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+    </row>
+    <row r="2" spans="2:13" ht="70.5" customHeight="1">
+      <c r="B2" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-    </row>
-    <row r="3" spans="2:12" ht="80.25" customHeight="1">
-      <c r="B3" s="67" t="s">
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="75"/>
+    </row>
+    <row r="3" spans="2:13" ht="80.25" customHeight="1">
+      <c r="B3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="72"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-    </row>
-    <row r="4" spans="2:12" ht="14.65" customHeight="1">
-      <c r="B4" s="69" t="s">
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="75"/>
+    </row>
+    <row r="4" spans="2:13" ht="14.65" customHeight="1">
+      <c r="B4" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="68" t="s">
+      <c r="C4" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="71" t="s">
+      <c r="E4" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71" t="s">
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-    </row>
-    <row r="5" spans="2:12" ht="30.75">
-      <c r="B5" s="70"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="32" t="s">
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="M4" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="32" t="s">
+    </row>
+    <row r="5" spans="2:13" ht="30.75">
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="33" t="s">
+      <c r="F5" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="G5" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="J5" s="33" t="s">
+      <c r="H5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="33" t="s">
+      <c r="I5" s="28" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" ht="60.75">
-      <c r="B6" s="59" t="s">
+      <c r="J5" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="K5" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="90" t="s">
+      <c r="L5" s="78"/>
+      <c r="M5" s="80"/>
+    </row>
+    <row r="6" spans="2:13" ht="60.75">
+      <c r="B6" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="26">
+      <c r="C6" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="110" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="19">
         <v>14</v>
       </c>
-      <c r="F6" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="28" t="s">
+      <c r="F6" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="28" t="s">
+      <c r="G6" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="29" t="s">
+      <c r="H6" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="30" t="s">
+      <c r="I6" s="22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="2:12">
-      <c r="B7" s="59"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="58"/>
-    </row>
-    <row r="8" spans="2:12" ht="165" customHeight="1">
-      <c r="B8" s="60"/>
-      <c r="C8" s="31" t="s">
+      <c r="J6" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="90" t="s">
+      <c r="K6" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="21">
+      <c r="L6" s="76" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13">
+      <c r="B7" s="50"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="76"/>
+      <c r="M7" s="32"/>
+    </row>
+    <row r="8" spans="2:13" ht="165" customHeight="1">
+      <c r="B8" s="51"/>
+      <c r="C8" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="110" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="19">
         <v>13</v>
       </c>
-      <c r="F8" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="22">
-        <v>0</v>
-      </c>
-      <c r="H8" s="22">
-        <v>0</v>
-      </c>
-      <c r="I8" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="J8" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="K8" s="25" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" ht="13.5" customHeight="1">
-      <c r="B9" s="60"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="57"/>
-      <c r="K9" s="58"/>
-    </row>
-    <row r="10" spans="2:12" ht="91.5">
-      <c r="B10" s="60"/>
-      <c r="C10" s="31" t="s">
+      <c r="F8" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="90" t="s">
+      <c r="G8" s="20">
+        <v>0</v>
+      </c>
+      <c r="H8" s="20">
+        <v>0</v>
+      </c>
+      <c r="I8" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="21">
+      <c r="J8" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="L8" s="76" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="13.5" customHeight="1">
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="76"/>
+      <c r="M9" s="32"/>
+    </row>
+    <row r="10" spans="2:13" ht="91.5">
+      <c r="B10" s="51"/>
+      <c r="C10" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="110" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="19">
         <v>16</v>
       </c>
-      <c r="F10" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="22">
-        <v>0</v>
-      </c>
-      <c r="H10" s="22">
-        <v>0</v>
-      </c>
-      <c r="I10" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="J10" s="28" t="s">
+      <c r="F10" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="20">
+        <v>0</v>
+      </c>
+      <c r="H10" s="20">
+        <v>0</v>
+      </c>
+      <c r="I10" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="K10" s="21">
+        <v>0</v>
+      </c>
+      <c r="L10" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="K10" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" ht="14.65" customHeight="1">
-      <c r="B11" s="18"/>
+      <c r="M10" s="32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" ht="14.65" customHeight="1">
+      <c r="B11" s="19"/>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
@@ -2831,163 +3137,165 @@
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>
-      <c r="K11" s="5"/>
-    </row>
-    <row r="12" spans="2:12"/>
-    <row r="13" spans="2:12"/>
-    <row r="14" spans="2:12" ht="14.65" customHeight="1">
-      <c r="B14" s="73" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="74"/>
-      <c r="I14" s="74"/>
-      <c r="J14" s="74"/>
-      <c r="K14" s="74"/>
-      <c r="L14" s="75"/>
-    </row>
-    <row r="15" spans="2:12">
-      <c r="B15" s="76" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="77"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="77"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="77"/>
-      <c r="J15" s="77"/>
-      <c r="K15" s="77"/>
-      <c r="L15" s="78"/>
-    </row>
-    <row r="16" spans="2:12">
+      <c r="K11" s="32"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="32"/>
+    </row>
+    <row r="12" spans="2:13"/>
+    <row r="13" spans="2:13"/>
+    <row r="14" spans="2:13" ht="14.65" customHeight="1">
+      <c r="B14" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="59"/>
+    </row>
+    <row r="15" spans="2:13">
+      <c r="B15" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="61"/>
+      <c r="L15" s="62"/>
+    </row>
+    <row r="16" spans="2:13">
       <c r="B16" s="13"/>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="49"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="15" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="L16" s="14" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="2:12" ht="30.75">
-      <c r="B17" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="51"/>
-      <c r="E17" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="23">
-        <v>0</v>
-      </c>
-      <c r="G17" s="22">
-        <v>0</v>
-      </c>
-      <c r="H17" s="23">
-        <v>0</v>
-      </c>
-      <c r="I17" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="J17" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="K17" s="21">
-        <v>0</v>
-      </c>
-      <c r="L17" s="21">
+      <c r="B17" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="46"/>
+      <c r="E17" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="21">
+        <v>0</v>
+      </c>
+      <c r="G17" s="20">
+        <v>0</v>
+      </c>
+      <c r="H17" s="21">
+        <v>0</v>
+      </c>
+      <c r="I17" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="J17" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="K17" s="19">
+        <v>0</v>
+      </c>
+      <c r="L17" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:12" ht="30.75">
-      <c r="B18" s="60"/>
-      <c r="C18" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="53"/>
-      <c r="E18" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="F18" s="23">
-        <v>0</v>
-      </c>
-      <c r="G18" s="23">
-        <v>0</v>
-      </c>
-      <c r="H18" s="23">
-        <v>0</v>
-      </c>
-      <c r="I18" s="23">
-        <v>0</v>
-      </c>
-      <c r="J18" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="K18" s="21">
-        <v>0</v>
-      </c>
-      <c r="L18" s="21">
+      <c r="B18" s="51"/>
+      <c r="C18" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="48"/>
+      <c r="E18" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="21">
+        <v>0</v>
+      </c>
+      <c r="G18" s="21">
+        <v>0</v>
+      </c>
+      <c r="H18" s="21">
+        <v>0</v>
+      </c>
+      <c r="I18" s="21">
+        <v>0</v>
+      </c>
+      <c r="J18" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="K18" s="19">
+        <v>0</v>
+      </c>
+      <c r="L18" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:12" ht="30.75">
-      <c r="B19" s="60"/>
-      <c r="C19" s="52" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="53"/>
-      <c r="E19" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="F19" s="23">
-        <v>0</v>
-      </c>
-      <c r="G19" s="23">
-        <v>0</v>
-      </c>
-      <c r="H19" s="23">
-        <v>0</v>
-      </c>
-      <c r="I19" s="23">
-        <v>0</v>
-      </c>
-      <c r="J19" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="K19" s="21">
-        <v>0</v>
-      </c>
-      <c r="L19" s="21">
+      <c r="B19" s="51"/>
+      <c r="C19" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="48"/>
+      <c r="E19" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="21">
+        <v>0</v>
+      </c>
+      <c r="G19" s="21">
+        <v>0</v>
+      </c>
+      <c r="H19" s="21">
+        <v>0</v>
+      </c>
+      <c r="I19" s="21">
+        <v>0</v>
+      </c>
+      <c r="J19" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="K19" s="19">
+        <v>0</v>
+      </c>
+      <c r="L19" s="19">
         <v>0</v>
       </c>
     </row>
@@ -3018,178 +3326,180 @@
       <c r="L21" s="17"/>
     </row>
     <row r="22" spans="2:12">
-      <c r="B22" s="73" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="74"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="74"/>
-      <c r="I22" s="74"/>
-      <c r="J22" s="74"/>
-      <c r="K22" s="74"/>
-      <c r="L22" s="75"/>
+      <c r="B22" s="57" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="58"/>
+      <c r="J22" s="58"/>
+      <c r="K22" s="58"/>
+      <c r="L22" s="59"/>
     </row>
     <row r="23" spans="2:12" ht="14.65" customHeight="1">
-      <c r="B23" s="61" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="63"/>
+      <c r="B23" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="54"/>
     </row>
     <row r="24" spans="2:12">
       <c r="B24" s="13"/>
-      <c r="C24" s="48" t="s">
+      <c r="C24" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="49"/>
+      <c r="D24" s="44"/>
       <c r="E24" s="15" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="K24" s="13" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="L24" s="14" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="30.75">
-      <c r="B25" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="51"/>
-      <c r="E25" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25" s="23">
-        <v>0</v>
-      </c>
-      <c r="G25" s="23">
-        <v>0</v>
-      </c>
-      <c r="H25" s="23">
-        <v>0</v>
-      </c>
-      <c r="I25" s="23">
-        <v>0</v>
-      </c>
-      <c r="J25" s="23">
-        <v>0</v>
-      </c>
-      <c r="K25" s="21">
-        <v>0</v>
-      </c>
-      <c r="L25" s="21">
+      <c r="B25" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="46"/>
+      <c r="E25" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="21">
+        <v>0</v>
+      </c>
+      <c r="G25" s="21">
+        <v>0</v>
+      </c>
+      <c r="H25" s="21">
+        <v>0</v>
+      </c>
+      <c r="I25" s="21">
+        <v>0</v>
+      </c>
+      <c r="J25" s="21">
+        <v>0</v>
+      </c>
+      <c r="K25" s="19">
+        <v>0</v>
+      </c>
+      <c r="L25" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:12">
-      <c r="B26" s="60"/>
-      <c r="C26" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="53"/>
-      <c r="E26" s="23">
-        <v>0</v>
-      </c>
-      <c r="F26" s="23">
-        <v>0</v>
-      </c>
-      <c r="G26" s="23">
-        <v>0</v>
-      </c>
-      <c r="H26" s="23">
-        <v>0</v>
-      </c>
-      <c r="I26" s="23">
-        <v>0</v>
-      </c>
-      <c r="J26" s="23">
-        <v>0</v>
-      </c>
-      <c r="K26" s="21">
-        <v>0</v>
-      </c>
-      <c r="L26" s="21">
+      <c r="B26" s="51"/>
+      <c r="C26" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="48"/>
+      <c r="E26" s="21">
+        <v>0</v>
+      </c>
+      <c r="F26" s="21">
+        <v>0</v>
+      </c>
+      <c r="G26" s="21">
+        <v>0</v>
+      </c>
+      <c r="H26" s="21">
+        <v>0</v>
+      </c>
+      <c r="I26" s="21">
+        <v>0</v>
+      </c>
+      <c r="J26" s="21">
+        <v>0</v>
+      </c>
+      <c r="K26" s="19">
+        <v>0</v>
+      </c>
+      <c r="L26" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:12">
-      <c r="B27" s="60"/>
-      <c r="C27" s="52" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" s="53"/>
-      <c r="E27" s="23">
-        <v>0</v>
-      </c>
-      <c r="F27" s="23">
-        <v>0</v>
-      </c>
-      <c r="G27" s="23">
-        <v>0</v>
-      </c>
-      <c r="H27" s="23">
-        <v>0</v>
-      </c>
-      <c r="I27" s="23">
-        <v>0</v>
-      </c>
-      <c r="J27" s="23">
-        <v>0</v>
-      </c>
-      <c r="K27" s="21">
-        <v>0</v>
-      </c>
-      <c r="L27" s="21">
+      <c r="B27" s="51"/>
+      <c r="C27" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="48"/>
+      <c r="E27" s="21">
+        <v>0</v>
+      </c>
+      <c r="F27" s="21">
+        <v>0</v>
+      </c>
+      <c r="G27" s="21">
+        <v>0</v>
+      </c>
+      <c r="H27" s="21">
+        <v>0</v>
+      </c>
+      <c r="I27" s="21">
+        <v>0</v>
+      </c>
+      <c r="J27" s="21">
+        <v>0</v>
+      </c>
+      <c r="K27" s="19">
+        <v>0</v>
+      </c>
+      <c r="L27" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:12">
-      <c r="E28" s="34"/>
+      <c r="E28" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="27">
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B23:L23"/>
     <mergeCell ref="C7:K7"/>
     <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="B2:K2"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="E4:G4"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="B6:B10"/>
-    <mergeCell ref="B3:K3"/>
     <mergeCell ref="B14:L14"/>
     <mergeCell ref="B15:L15"/>
     <mergeCell ref="B22:L22"/>
@@ -3211,10 +3521,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03285090-925E-4318-9A54-5659E6D310C9}">
-  <dimension ref="C1:J15"/>
+  <dimension ref="C1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
@@ -3227,158 +3537,237 @@
     <col min="8" max="8" width="19.7109375" customWidth="1"/>
     <col min="9" max="9" width="33.42578125" customWidth="1"/>
     <col min="10" max="10" width="31.140625" customWidth="1"/>
+    <col min="11" max="11" width="48" customWidth="1"/>
+    <col min="12" max="12" width="25.140625" customWidth="1"/>
+    <col min="13" max="13" width="60.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:10" ht="15"/>
-    <row r="2" spans="3:10" ht="15"/>
-    <row r="3" spans="3:10" ht="15">
-      <c r="C3" s="79" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-    </row>
-    <row r="4" spans="3:10" ht="14.65" customHeight="1">
-      <c r="C4" s="80" t="s">
+    <row r="1" spans="3:13" ht="15"/>
+    <row r="2" spans="3:13" ht="45.75" customHeight="1">
+      <c r="C2" s="82" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="82"/>
+    </row>
+    <row r="3" spans="3:13" ht="54" customHeight="1">
+      <c r="C3" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+    </row>
+    <row r="4" spans="3:13" ht="15">
+      <c r="C4" s="81" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="89" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" s="86" t="s">
+        <v>66</v>
+      </c>
+      <c r="M4" s="86" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" ht="14.65" customHeight="1">
+      <c r="C5" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="80" t="s">
+      <c r="D5" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="81" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="83" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" s="85" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" s="85"/>
-      <c r="I4" s="85"/>
-      <c r="J4" s="85"/>
-    </row>
-    <row r="5" spans="3:10" ht="14.65" customHeight="1">
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="82"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="I5" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="J5" s="41" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="3:10" ht="96" customHeight="1">
-      <c r="C6" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="27">
+      <c r="E5" s="64" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="89"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="86"/>
+    </row>
+    <row r="6" spans="3:13" ht="14.65" customHeight="1">
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="87" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="87" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="88" t="s">
+        <v>71</v>
+      </c>
+      <c r="J6" s="88" t="s">
+        <v>72</v>
+      </c>
+      <c r="K6" s="89"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="86"/>
+    </row>
+    <row r="7" spans="3:13" ht="96" customHeight="1">
+      <c r="C7" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" s="43">
-        <v>0</v>
-      </c>
-      <c r="H6" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" s="43">
-        <v>0</v>
-      </c>
-      <c r="J6" s="42" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="3:10" ht="60.75">
-      <c r="C7" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" s="23">
+      <c r="E7" s="25">
+        <v>18</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" s="90">
+        <v>0</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="90">
+        <v>0</v>
+      </c>
+      <c r="J7" s="92" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="L7" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="M7" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" ht="86.25" customHeight="1">
+      <c r="C8" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="21">
         <v>15</v>
       </c>
-      <c r="F7" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G7" s="43">
-        <v>0</v>
-      </c>
-      <c r="H7" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="I7" s="43">
-        <v>0</v>
-      </c>
-      <c r="J7" s="43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="3:10" ht="106.5">
-      <c r="C8" s="44" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="23">
+      <c r="F8" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="36">
+        <v>0</v>
+      </c>
+      <c r="H8" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8" s="84">
+        <v>0</v>
+      </c>
+      <c r="J8" s="36">
+        <v>0</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="L8" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" ht="106.5">
+      <c r="C9" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="21">
         <v>21</v>
       </c>
-      <c r="F8" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="G8" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="H8" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="I8" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="J8" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="3:10" ht="15"/>
-    <row r="11" spans="3:10" ht="14.65" customHeight="1">
-      <c r="E11" s="17"/>
-      <c r="G11" s="20"/>
-    </row>
-    <row r="12" spans="3:10" ht="14.65" customHeight="1"/>
-    <row r="13" spans="3:10" ht="15"/>
-    <row r="14" spans="3:10" ht="15"/>
-    <row r="15" spans="3:10" ht="15">
-      <c r="E15" s="17"/>
-      <c r="G15" s="20"/>
+      <c r="F9" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9" s="42">
+        <v>0</v>
+      </c>
+      <c r="K9" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="L9" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="M9" s="19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" ht="15"/>
+    <row r="12" spans="3:13" ht="14.65" customHeight="1">
+      <c r="E12" s="17"/>
+      <c r="G12" s="18"/>
+    </row>
+    <row r="13" spans="3:13" ht="14.65" customHeight="1"/>
+    <row r="14" spans="3:13" ht="15"/>
+    <row r="15" spans="3:13" ht="15"/>
+    <row r="16" spans="3:13" ht="15">
+      <c r="E16" s="17"/>
+      <c r="G16" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C3:J3"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:J4"/>
+  <mergeCells count="11">
+    <mergeCell ref="C2:M2"/>
+    <mergeCell ref="C3:M3"/>
+    <mergeCell ref="K4:K6"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="C4:J4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3404,24 +3793,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:10">
-      <c r="C1" s="86" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
+      <c r="C1" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
     <row r="2" spans="3:10">
-      <c r="C2" s="87" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
+      <c r="C2" s="67" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -3438,30 +3827,30 @@
         <v>5</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="3:10">
       <c r="C5" s="7"/>
       <c r="D5" s="8" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="9"/>
     </row>
     <row r="6" spans="3:10">
       <c r="C6" s="1" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="D6" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="3:10">
       <c r="C7" s="3"/>
       <c r="D7" s="4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="5"/>
@@ -3477,10 +3866,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC2638F1-068A-4418-89AB-4E730123006C}">
-  <dimension ref="B1:I19"/>
+  <dimension ref="B1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65"/>
@@ -3493,145 +3882,223 @@
     <col min="7" max="7" width="63.140625" customWidth="1"/>
     <col min="8" max="8" width="36.5703125" customWidth="1"/>
     <col min="9" max="9" width="53" customWidth="1"/>
+    <col min="10" max="10" width="49.42578125" customWidth="1"/>
+    <col min="11" max="11" width="61.140625" customWidth="1"/>
+    <col min="12" max="12" width="68.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15"/>
-    <row r="2" spans="2:9" ht="15"/>
-    <row r="3" spans="2:9" ht="15"/>
-    <row r="4" spans="2:9" ht="15">
-      <c r="B4" s="88" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="88"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="88"/>
-    </row>
-    <row r="5" spans="2:9" ht="15">
-      <c r="B5" s="80" t="s">
+    <row r="1" spans="2:12" ht="15"/>
+    <row r="2" spans="2:12" ht="56.25" customHeight="1">
+      <c r="B2" s="93" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="94"/>
+      <c r="I2" s="94"/>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94"/>
+      <c r="L2" s="95"/>
+    </row>
+    <row r="3" spans="2:12" ht="46.5" customHeight="1">
+      <c r="B3" s="108" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="97"/>
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="98"/>
+    </row>
+    <row r="4" spans="2:12" ht="15">
+      <c r="B4" s="81" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="81"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="105" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" s="102" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="99" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="15">
+      <c r="B5" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="80" t="s">
+      <c r="C5" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="89" t="s">
-        <v>82</v>
-      </c>
-      <c r="E5" s="80" t="s">
-        <v>57</v>
-      </c>
-      <c r="F5" s="85" t="s">
-        <v>58</v>
-      </c>
-      <c r="G5" s="85"/>
-      <c r="H5" s="85"/>
-      <c r="I5" s="85"/>
-    </row>
-    <row r="6" spans="2:9" ht="30.95" customHeight="1">
-      <c r="B6" s="80"/>
-      <c r="C6" s="80"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="H6" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="I6" s="47" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="145.5" customHeight="1">
-      <c r="B7" s="35" t="s">
+      <c r="D5" s="68" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="65" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="106"/>
+      <c r="K5" s="103"/>
+      <c r="L5" s="100"/>
+    </row>
+    <row r="6" spans="2:12" ht="30.95" customHeight="1">
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="I6" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="J6" s="107"/>
+      <c r="K6" s="104"/>
+      <c r="L6" s="101"/>
+    </row>
+    <row r="7" spans="2:12" ht="145.5" customHeight="1">
+      <c r="B7" s="109" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="90">
+        <v>18</v>
+      </c>
+      <c r="E7" s="90" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7" s="91" t="s">
+        <v>109</v>
+      </c>
+      <c r="J7" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="K7" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="153.75" customHeight="1">
+      <c r="B8" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="36">
+        <v>15</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="H8" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="I8" s="83" t="s">
+        <v>116</v>
+      </c>
+      <c r="J8" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="43">
-        <v>18</v>
-      </c>
-      <c r="E7" s="43" t="s">
-        <v>85</v>
-      </c>
-      <c r="F7" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="G7" s="42" t="s">
+      <c r="K8" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="192.75" customHeight="1">
+      <c r="B9" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="H7" s="42" t="s">
-        <v>88</v>
-      </c>
-      <c r="I7" s="42" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" ht="153.75" customHeight="1">
-      <c r="B8" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="C8" s="37" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="43">
-        <v>15</v>
-      </c>
-      <c r="E8" s="43" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8" s="42" t="s">
+      <c r="D9" s="36">
+        <v>21</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="I9" s="96" t="s">
+        <v>123</v>
+      </c>
+      <c r="J9" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="G8" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="H8" s="42" t="s">
-        <v>94</v>
-      </c>
-      <c r="I8" s="42" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="192.75" customHeight="1">
-      <c r="B9" s="35" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" s="37" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" s="43">
-        <v>21</v>
-      </c>
-      <c r="E9" s="43" t="s">
-        <v>97</v>
-      </c>
-      <c r="F9" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" ht="15"/>
-    <row r="16" spans="2:9" ht="15"/>
+      <c r="K9" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="19" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="15"/>
+    <row r="16" spans="2:12" ht="15"/>
     <row r="17" ht="15"/>
     <row r="19" ht="15"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="11">
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="K4:K6"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B3:L3"/>
     <mergeCell ref="F5:I5"/>
     <mergeCell ref="B4:I4"/>
     <mergeCell ref="B5:B6"/>
@@ -3661,20 +4128,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5">
-      <c r="B1" s="86" t="s">
-        <v>55</v>
-      </c>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
+      <c r="B1" s="66" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
     </row>
     <row r="2" spans="2:5">
-      <c r="B2" s="87" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
+      <c r="B2" s="67" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
     </row>
     <row r="4" spans="2:5">
       <c r="B4" s="10" t="s">
@@ -3687,30 +4154,30 @@
         <v>5</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="2:5">
       <c r="B5" s="7"/>
       <c r="C5" s="8" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="1" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="2:5">
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="5"/>

</xml_diff>